<commit_message>
v2.1 updated according to srs
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_PUBLISHVIDEO.xlsx
+++ b/LH_TESTCASES/LH_TC_PUBLISHVIDEO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\LH_TEMPLATES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\oooo\Group-3-Learning-hub-dev\LH_TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_PUPLISHVIDEO" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="120">
   <si>
     <t>Preconditions</t>
   </si>
@@ -181,55 +181,6 @@
     <t>Verify error if no title is entered</t>
   </si>
   <si>
-    <t>1. Open website without logging in
-2. Try to access the publish page</t>
-  </si>
-  <si>
-    <t>1. Log in to the system
-2. Confirm 'Categories' page is accessible</t>
-  </si>
-  <si>
-    <t>1. Open 'Categories' page
-2. Open dropdown menu
-3. Check for 'Publish video' option</t>
-  </si>
-  <si>
-    <t>1. Select 'Publish video' from the dropdown</t>
-  </si>
-  <si>
-    <t>1. Open publish video page
-2. Select a video file
-3. Observe size indicator</t>
-  </si>
-  <si>
-    <t>1. Open upload file window
-2. Check allowed file types in the browser</t>
-  </si>
-  <si>
-    <t>1. Upload video file &gt;100MB
-2. Check if publish button is enabled</t>
-  </si>
-  <si>
-    <t>1. Upload valid video
-2. Leave title empty
-3. Attempt to publish</t>
-  </si>
-  <si>
-    <t>1. Upload valid video
-2. Enter a valid title
-3. Click publish</t>
-  </si>
-  <si>
-    <t>1. Leave video upload field empty
-2. Enter a title
-3. Click publish</t>
-  </si>
-  <si>
-    <t>1. Upload valid video
-2. Leave title empty
-3. Click publish</t>
-  </si>
-  <si>
     <t>User is redirected to login page or access is denied</t>
   </si>
   <si>
@@ -245,34 +196,18 @@
     <t>Video size indicator is shown in format like: 5MB/100MB</t>
   </si>
   <si>
-    <t>Only MP4 files are visible in the file browser</t>
-  </si>
-  <si>
     <t>Publish button is disabled for videos &gt;100MB</t>
   </si>
   <si>
     <t>Publish button is disabled when title is empty</t>
   </si>
   <si>
-    <t>Video is saved to the database and linked to the selected category</t>
-  </si>
-  <si>
     <t>Error message displayed: 'Please Upload a valid video'</t>
   </si>
   <si>
     <t>Error message displayed: 'Please add a title'</t>
   </si>
   <si>
-    <t>1. User opens the browser.
-2. Navigates to the website.</t>
-  </si>
-  <si>
-    <t>1. User opens the browser. 
-2. Navigates to the website. 
-3. Logs in as a default user and
- goes to the home page.</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -285,20 +220,6 @@
     <t>Upload Valid Video File (&lt;100MB)</t>
   </si>
   <si>
-    <t>1. User opens the browser.
-2. Navigates to the website.
-3. Logs in as a default user and goes to the home page.</t>
-  </si>
-  <si>
-    <t>1. Open publishing interface.
-2. Click "Upload Video."
-3. Select 90MB MP4 file.
-4. Click "Publish."</t>
-  </si>
-  <si>
-    <t>Valid Video: 90MB MP4</t>
-  </si>
-  <si>
     <t>File uploads successfully.</t>
   </si>
   <si>
@@ -308,30 +229,12 @@
     <t>Upload Valid Video File (=100MB)</t>
   </si>
   <si>
-    <t>1. Open publishing interface.
-2. Click "Upload Video."
-3. Select 100MB MP4 file.
-4. Click "Publish."</t>
-  </si>
-  <si>
-    <t>Valid Video: 100MB MP4</t>
-  </si>
-  <si>
     <t>LH-TC-PUBLISHVIDEO-003</t>
   </si>
   <si>
     <t>Upload Invalid Video File (&gt;100MB)</t>
   </si>
   <si>
-    <t>1. Open publishing interface.
-2. Click "Upload Video."
-3. Select 110MB MP4 file.
-4. Click "Publish."</t>
-  </si>
-  <si>
-    <t>Invalid Video: 110MB MP4</t>
-  </si>
-  <si>
     <t>File is rejected, with error message of: "Max size: 100MB."</t>
   </si>
   <si>
@@ -344,54 +247,242 @@
     <t>Validate Valid Video Format (.mp4 Only)</t>
   </si>
   <si>
-    <t>Valid Video Format: sample.mp4</t>
-  </si>
-  <si>
     <t>LH-TC-PUBLISHVIDEO-005</t>
   </si>
   <si>
     <t>Validate Invalid Video Format (e.g., .avi)</t>
   </si>
   <si>
-    <t>1. Open publishing interface.
-2. Click "Upload Video."
-3. Select 90MB AVI file.
-4. Click "Publish."</t>
-  </si>
-  <si>
-    <t>Invalid Video Format: sample.avi</t>
-  </si>
-  <si>
     <t>File is rejected with error: "Only MP4 format is allowed."</t>
   </si>
   <si>
-    <t>Video File: sample_large.mp4 (110MB)</t>
-  </si>
-  <si>
-    <t>Video File: sample_small.mp4 (90MB)
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Hala Eldaly</t>
+  </si>
+  <si>
+    <t>updated according to srs</t>
+  </si>
+  <si>
+    <t>Only MP4 files are visible in the PC</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>PUBLISH VIDEO</t>
+  </si>
+  <si>
+    <t>LH-TC-PUBLISHVIDEO-017</t>
+  </si>
+  <si>
+    <t>Verify publish button is disabled for &lt;100MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The publish button is available </t>
+  </si>
+  <si>
+    <t>LH-TC-PUBLISHVIDEO-018</t>
+  </si>
+  <si>
+    <t>Verify publish button is disabled for =100MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User Navigates the browser url , without logging in
+</t>
+  </si>
+  <si>
+    <t>1. User Navigates the browser url.
+2. Login with valid email and password
+3. Navigates to the [UserHome]
+4. Go to categories page
+5. Select Publish video option from dropdown list for puplishing 
+6. Select 90MB MP4 file to upload.
+7. Enter video title
+8. Click "Publish."</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Valid Video: 90MB MP4</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Valid Video: 100MB MP4</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Invalid Video: 110MB MP4</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Valid Video Format: sample.mp4</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Invalid Video Format: sample.avi</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Video File: sample_large.mp4 (110MB)</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Video File: sample_large.mp4 (80MB)</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Video File: sample_large.mp4 (100MB)</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Video File: sample_small.mp4 (90MB)
 Title: (empty)</t>
   </si>
   <si>
-    <t>Title: "Test Video"
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Title: "Test Video"
+Video: valid sample video</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword123
+Title: "Test Video"
 Video: (none)</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Hala Eldaly</t>
-  </si>
-  <si>
-    <t>V2.0</t>
-  </si>
-  <si>
-    <t>updated according to srs</t>
+    <t>Video is saved to the database and linked to the 
+selected category</t>
+  </si>
+  <si>
+    <t>1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option.
+6. Select 90MB MP4 file to upload.
+7. Enter video title
+8. Click "Publish."</t>
+  </si>
+  <si>
+    <t>1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option.
+6. Select 100MB MP4 file to upload.
+7. Enter video title
+8. Click "Publish."</t>
+  </si>
+  <si>
+    <t>1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option. 
+6. Select 110MB MP4 file to upload.
+7. Enter video title
+8. Click "Publish."</t>
+  </si>
+  <si>
+    <t>1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option.
+6. Select 90MB avi file to upload.
+7. Enter video title
+8. Click "Publish."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. navigate a dropdown list for puplishing </t>
+  </si>
+  <si>
+    <t>1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option.
+6. Observe size indicator</t>
+  </si>
+  <si>
+    <t>1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option.
+6. Select 90MB MP4 file to upload.
+7. Enter video title
+8. Click "Publish."</t>
+  </si>
+  <si>
+    <t>1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option.
+6. Select 90MB MP4 file to upload.
+7. Click "Publish."</t>
+  </si>
+  <si>
+    <t>1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option.
+5.  Enter video title
+6. Click "Publish."</t>
+  </si>
+  <si>
+    <t>User is logged in , navigates to User Home Page , categories page , puplish video page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User isn't logged in </t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>v2.1</t>
   </si>
 </sst>
 </file>
@@ -422,14 +513,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -450,8 +533,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,8 +554,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -571,14 +667,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -590,43 +724,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -637,17 +753,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -988,19 +1185,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="63" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="73.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="76.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="45.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="79.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
@@ -1014,37 +1211,43 @@
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1088,473 +1291,544 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+    <row r="9" spans="1:10" s="15" customFormat="1" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="24" t="s">
+    </row>
+    <row r="10" spans="1:10" s="15" customFormat="1" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="24" t="s">
+    </row>
+    <row r="13" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.35">
+      <c r="A15" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="25"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="168" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="24" t="s">
+    </row>
+    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.35">
+      <c r="A17" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="25"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="168" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="12"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="24" t="s">
+      <c r="H19" s="25"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="210" x14ac:dyDescent="0.35">
+      <c r="A20" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="F20" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="12"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="24" t="s">
+    </row>
+    <row r="21" spans="1:10" ht="231" x14ac:dyDescent="0.35">
+      <c r="A21" s="30"/>
+      <c r="B21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="189" x14ac:dyDescent="0.35">
+      <c r="A22" s="31"/>
+      <c r="B22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="120" x14ac:dyDescent="0.35">
+      <c r="A23" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="25"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="210" x14ac:dyDescent="0.35">
+      <c r="A24" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" s="12"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="120" x14ac:dyDescent="0.35">
+      <c r="A25" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="24"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="C25" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="25"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="24" t="s">
+    </row>
+    <row r="26" spans="1:10" ht="189" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A15" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A18" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A20" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="24" t="s">
+      <c r="C26" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A21" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="H21" s="12"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A22" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="25" t="s">
+      <c r="G26" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A24" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I25" s="27"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I27" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A8:I9"/>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A9:A11"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:I13 I15:I1048576">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="I9:I13 I15:I20 I23:I1048576">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I14)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I22)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I14)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pass",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1571,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,25 +1871,33 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" s="8" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="D2" s="13">
         <v>45789</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+    <row r="3" spans="1:4" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="13">
+        <v>45789</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>

</xml_diff>

<commit_message>
v2.3 Updated the TCs according to CRS
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_PUBLISHVIDEO.xlsx
+++ b/LH_TESTCASES/LH_TC_PUBLISHVIDEO.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Desktop\Group-3-Learning-hub-dev (5)\Group-3-Learning-hub-dev\LH_TESTCASES\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457619D1-6AFF-457B-AEBD-20DE3B60ABF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_PUPLISHVIDEO" sheetId="1" r:id="rId1"/>
@@ -37,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="165">
   <si>
     <t>Project name</t>
   </si>
@@ -510,7 +504,94 @@
     <t>Verify error if no title is entered</t>
   </si>
   <si>
-    <t>Error message displayed: 'Please add a title'</t>
+    <t>Error message displayed: 'Title is required'</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-014</t>
+  </si>
+  <si>
+    <t>LH-TC-PUBLISHVIDEO-019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the system accepts titles with fewer than 40 characters
+</t>
+  </si>
+  <si>
+    <t>1. Open the browser and navigate to the application URL.
+2. Log in using valid email and password.
+3. Go to the User Home page.
+4. Navigate to the Categories page.
+5. From the dropdown, select the "Publish Video" option.
+4. Enter a title within the allowed limit
+6. Upload a video within the allowed limit
+7. Click "Publish."</t>
+  </si>
+  <si>
+    <t>Title: "We are just testing"</t>
+  </si>
+  <si>
+    <t>The system should allow input of a title with a length of less than 40 characters</t>
+  </si>
+  <si>
+    <t>The system successfully allow input of a title with a length of less than 40 characters</t>
+  </si>
+  <si>
+    <t>LH-TC-PUBLISHVIDEO-020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the system accepts titles with the exact length of 40 characters
+</t>
+  </si>
+  <si>
+    <t>Title: "Hi there, we are just testing the length"</t>
+  </si>
+  <si>
+    <t>The system uploads the video successfully without any issues</t>
+  </si>
+  <si>
+    <t>The system uploads the video successfully</t>
+  </si>
+  <si>
+    <t>LH-TC-PUBLISHVIDEO-021</t>
+  </si>
+  <si>
+    <t>Verify that the system rejects titles exceeding 40 characters</t>
+  </si>
+  <si>
+    <t>Title: "We are just testing the new title constraints"</t>
+  </si>
+  <si>
+    <t>The system display an error message: "Title too long" and disables the publish button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An error message appears " Title too long" and publish button is disabled </t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-015</t>
+  </si>
+  <si>
+    <t>LH-TC-PUBLISHVIDEO-022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify that the system collapses multiple consecutive spaces into a single space in the title</t>
+  </si>
+  <si>
+    <t>Title: "Learning                   Hub"</t>
+  </si>
+  <si>
+    <t>The system uploads the video successfully without any issues or extra spaces</t>
+  </si>
+  <si>
+    <t>The system uploads the video successfully without any extra spaces</t>
+  </si>
+  <si>
+    <t>LH-TC-PUBLISHVIDEO-023</t>
+  </si>
+  <si>
+    <t>Verify that the system rejects a title consisting only of spaces</t>
+  </si>
+  <si>
+    <t>Title: "                             "</t>
   </si>
   <si>
     <t>Version number</t>
@@ -541,13 +622,25 @@
   </si>
   <si>
     <t>Executed TCs</t>
+  </si>
+  <si>
+    <t>v2.3</t>
+  </si>
+  <si>
+    <t>Added new TCs according to change request</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,21 +652,21 @@
       <sz val="20"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -581,44 +674,188 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,18 +864,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
+        <fgColor theme="3" tint="0.399945066682943"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799951170384838"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -770,24 +1187,280 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color theme="0"/>
+        <color rgb="FFB2B2B2"/>
       </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
       <bottom style="thin">
-        <color theme="0"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -807,6 +1480,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -822,6 +1504,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -834,81 +1519,107 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="26" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -957,9 +1668,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1246,820 +1954,1071 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="37.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="49.88671875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="67.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="61.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="34.88671875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="29.6640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="21.109375" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="29.8857142857143" style="14" customWidth="1"/>
+    <col min="2" max="2" width="37.552380952381" style="15" customWidth="1"/>
+    <col min="3" max="3" width="49.8857142857143" style="15" customWidth="1"/>
+    <col min="4" max="4" width="57.6666666666667" style="15" customWidth="1"/>
+    <col min="5" max="5" width="57.3333333333333" style="15" customWidth="1"/>
+    <col min="6" max="6" width="38.552380952381" style="15" customWidth="1"/>
+    <col min="7" max="7" width="67.3333333333333" style="15" customWidth="1"/>
+    <col min="8" max="8" width="61.6666666666667" style="13" customWidth="1"/>
+    <col min="9" max="9" width="34.8857142857143" style="16" customWidth="1"/>
+    <col min="10" max="10" width="29.6666666666667" style="15" customWidth="1"/>
+    <col min="11" max="11" width="21.1047619047619" style="15" customWidth="1"/>
+    <col min="12" max="16384" width="9.1047619047619" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="66.75" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="11" customFormat="1" ht="66.75" customHeight="1" spans="1:8">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="9" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="9" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="9" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="25.8">
-      <c r="A8" s="10" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="9:9">
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="9:9">
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" spans="9:9">
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" s="12" customFormat="1" ht="26.25" spans="1:10">
+      <c r="A8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="126" customHeight="1">
-      <c r="A9" s="39" t="s">
+    <row r="9" s="13" customFormat="1" ht="126" customHeight="1" spans="1:10">
+      <c r="A9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="129" customHeight="1">
-      <c r="A10" s="40"/>
-      <c r="B10" s="13" t="s">
+    <row r="10" s="13" customFormat="1" ht="129" customHeight="1" spans="1:10">
+      <c r="A10" s="31"/>
+      <c r="B10" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="124.05" customHeight="1">
-      <c r="A11" s="41"/>
-      <c r="B11" s="13" t="s">
+    <row r="11" s="13" customFormat="1" ht="124.05" customHeight="1" spans="1:10">
+      <c r="A11" s="32"/>
+      <c r="B11" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A12" s="31" t="s">
+    <row r="12" s="13" customFormat="1" ht="53.25" customHeight="1" spans="1:10">
+      <c r="A12" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="34" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="17" t="s">
+    <row r="13" s="13" customFormat="1" ht="53.25" customHeight="1" spans="1:10">
+      <c r="A13" s="36"/>
+      <c r="B13" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="34" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A14" s="16" t="s">
+    <row r="14" s="13" customFormat="1" ht="53.25" customHeight="1" spans="1:10">
+      <c r="A14" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="78">
-      <c r="A15" s="17" t="s">
+    <row r="15" ht="78.75" spans="1:10">
+      <c r="A15" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="93.6">
-      <c r="A16" s="16" t="s">
+    <row r="16" ht="94.5" spans="1:10">
+      <c r="A16" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="48" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="78">
-      <c r="A17" s="17" t="s">
+    <row r="17" ht="78.75" spans="1:10">
+      <c r="A17" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="93.6">
-      <c r="A18" s="16" t="s">
+    <row r="18" ht="94.5" spans="1:10">
+      <c r="A18" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="J18" s="48" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="63" customHeight="1">
-      <c r="A19" s="17" t="s">
+    <row r="19" ht="63" customHeight="1" spans="1:10">
+      <c r="A19" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="20" t="s">
+      <c r="J19" s="47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="124.8">
-      <c r="A20" s="33" t="s">
+    <row r="20" ht="126" spans="1:10">
+      <c r="A20" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="J20" s="48" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="124.8">
-      <c r="A21" s="34"/>
-      <c r="B21" s="16" t="s">
+    <row r="21" ht="126" spans="1:10">
+      <c r="A21" s="38"/>
+      <c r="B21" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="21" t="s">
+      <c r="J21" s="48" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="140.4">
-      <c r="A22" s="35"/>
-      <c r="B22" s="16" t="s">
+    <row r="22" ht="141.75" spans="1:10">
+      <c r="A22" s="39"/>
+      <c r="B22" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="21" t="s">
+      <c r="J22" s="48" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="109.2">
-      <c r="A23" s="17" t="s">
+    <row r="23" ht="110.25" spans="1:10">
+      <c r="A23" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="47" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="124.8">
-      <c r="A24" s="16" t="s">
+    <row r="24" ht="126" spans="1:10">
+      <c r="A24" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="21" t="s">
+      <c r="J24" s="48" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="109.2">
-      <c r="A25" s="17" t="s">
+    <row r="25" ht="110.25" spans="1:10">
+      <c r="A25" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="I25" s="19" t="s">
+      <c r="I25" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J25" s="20" t="s">
+      <c r="J25" s="47" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="109.2">
-      <c r="A26" s="16" t="s">
+    <row r="26" ht="110.25" spans="1:10">
+      <c r="A26" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="G26" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="I26" s="19" t="s">
+      <c r="I26" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="21" t="s">
+      <c r="J26" s="48" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="I27" s="22"/>
+    <row r="27" ht="126" spans="1:10">
+      <c r="A27" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="I27" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" ht="126" spans="1:10">
+      <c r="A28" s="41"/>
+      <c r="B28" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G28" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="I28" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" s="48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" ht="126" spans="1:10">
+      <c r="A29" s="42"/>
+      <c r="B29" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="I29" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" ht="126" spans="1:10">
+      <c r="A30" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I30" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" ht="126" spans="1:10">
+      <c r="A31" s="45"/>
+      <c r="B31" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" s="48" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:I26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="7">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A20:A22"/>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A8:I26" etc:filterBottomFollowUsedRange="0">
+    <extLst/>
+  </autoFilter>
+  <mergeCells count="9">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A31"/>
   </mergeCells>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="containsText" dxfId="0" priority="25" operator="between" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="24" operator="between" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="23" operator="between" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",I27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="22" operator="between" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",I27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="21" operator="between" text="not executed">
+      <formula>NOT(ISERROR(SEARCH("not executed",I27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="containsText" dxfId="0" priority="20" operator="between" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="19" operator="between" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="18" operator="between" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",I28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="17" operator="between" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",I28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="16" operator="between" text="not executed">
+      <formula>NOT(ISERROR(SEARCH("not executed",I28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="containsText" dxfId="0" priority="15" operator="between" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="14" operator="between" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="13" operator="between" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",I29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="12" operator="between" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",I29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="11" operator="between" text="not executed">
+      <formula>NOT(ISERROR(SEARCH("not executed",I29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="containsText" dxfId="0" priority="10" operator="between" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="9" operator="between" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="8" operator="between" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",I30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="7" operator="between" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",I30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="between" text="not executed">
+      <formula>NOT(ISERROR(SEARCH("not executed",I30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="between" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="between" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="between" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",I31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="between" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",I31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="1" operator="between" text="not executed">
+      <formula>NOT(ISERROR(SEARCH("not executed",I31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I9:I26">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="not executed">
+    <cfRule type="containsText" dxfId="4" priority="26" operator="between" text="not executed">
       <formula>NOT(ISERROR(SEARCH("not executed",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="3" priority="27" operator="between" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="2" priority="28" operator="between" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I1048576">
-    <cfRule type="containsText" dxfId="1" priority="10" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="I9:I26 I32:I1048576">
+    <cfRule type="containsText" dxfId="1" priority="35" operator="between" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="11" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="0" priority="36" operator="between" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I27 I28 I29 I30 I31 I9:I26 I32:I1048576">
       <formula1>"Pass, Fail, Blocked, N/A"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="28"/>
+    <col min="1" max="1" width="31.6666666666667" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.3333333333333" style="4" customWidth="1"/>
+    <col min="3" max="3" width="39.8571428571429" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.1047619047619" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="26" customFormat="1" ht="25.8">
-      <c r="A1" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="27" customFormat="1" ht="42">
-      <c r="A2" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="24" t="s">
+    <row r="1" s="1" customFormat="1" ht="27" spans="1:4">
+      <c r="A1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="42.75" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" s="25">
+      <c r="C2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="7">
         <v>45789</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="27" customFormat="1" ht="42">
-      <c r="A3" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="24" t="s">
+    <row r="3" s="2" customFormat="1" ht="42" spans="1:4">
+      <c r="A3" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="25">
+      <c r="C3" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="7">
         <v>45789</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21">
-      <c r="A4" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="25">
+    <row r="4" ht="21" spans="1:4">
+      <c r="A4" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="7">
         <v>45793</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
+    <row r="5" ht="42" spans="1:4">
+      <c r="A5" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="7">
+        <v>45794</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-    </row>
-    <row r="7" spans="1:4" s="30" customFormat="1">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" s="3" customFormat="1" ht="15.75" spans="1:4">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>